<commit_message>
Updated excel testfile to default values
</commit_message>
<xml_diff>
--- a/tests/TestUtils/TestFiles/TestWorkbook_Excel_openpyxl.xlsx
+++ b/tests/TestUtils/TestFiles/TestWorkbook_Excel_openpyxl.xlsx
@@ -17,9 +17,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -59,7 +60,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -69,6 +70,8 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,18 +529,18 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Foo</t>
+          <t>Hello</t>
         </is>
       </c>
       <c r="C2" s="6" t="n">
-        <v>45852.39583333334</v>
+        <v>45213</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -552,18 +555,18 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bar</t>
+          <t>World</t>
         </is>
       </c>
       <c r="C3" s="6" t="n">
-        <v>45853.44809027778</v>
+        <v>45214.75</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -573,15 +576,15 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tschüss</t>
+          <t>Bye</t>
         </is>
       </c>
       <c r="C4" s="6" t="n">
-        <v>45854.50034722222</v>
+        <v>45215.83333333334</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -589,15 +592,15 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3.141</v>
+        <v>4.27</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Infinite Void</t>
+          <t>Outer Space</t>
         </is>
       </c>
       <c r="C5" s="6" t="n">
-        <v>45855.56788194444</v>
+        <v>45216</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -659,18 +662,18 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Foo</t>
+          <t>Hello</t>
         </is>
       </c>
       <c r="C2" s="6" t="n">
-        <v>45852.39583333334</v>
+        <v>45213</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -685,18 +688,18 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bar</t>
+          <t>World</t>
         </is>
       </c>
       <c r="C3" s="6" t="n">
-        <v>45853.44809027778</v>
+        <v>45214.75</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -706,15 +709,15 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tschüss</t>
+          <t>Bye</t>
         </is>
       </c>
       <c r="C4" s="6" t="n">
-        <v>45854.50034722222</v>
+        <v>45215.83333333334</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -722,15 +725,15 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3.141</v>
+        <v>4.27</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Infinite Void</t>
+          <t>Outer Space</t>
         </is>
       </c>
       <c r="C5" s="6" t="n">
-        <v>45855.56788194444</v>
+        <v>45216</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -828,18 +831,18 @@
     </row>
     <row r="5">
       <c r="B5" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Foo</t>
+          <t>Hello</t>
         </is>
       </c>
       <c r="D5" s="6" t="n">
-        <v>45852.39583333334</v>
+        <v>45213</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -854,18 +857,18 @@
     </row>
     <row r="6">
       <c r="B6" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bar</t>
+          <t>World</t>
         </is>
       </c>
       <c r="D6" s="6" t="n">
-        <v>45853.44809027778</v>
+        <v>45214.75</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -875,15 +878,15 @@
     </row>
     <row r="7">
       <c r="B7" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tschüss</t>
+          <t>Bye</t>
         </is>
       </c>
       <c r="D7" s="6" t="n">
-        <v>45854.50034722222</v>
+        <v>45215.83333333334</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -891,15 +894,15 @@
     </row>
     <row r="8">
       <c r="B8" t="n">
-        <v>3.141</v>
+        <v>4.27</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Infinite Void</t>
+          <t>Outer Space</t>
         </is>
       </c>
       <c r="D8" s="6" t="n">
-        <v>45855.56788194444</v>
+        <v>45216</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>

</xml_diff>